<commit_message>
get the random model
</commit_message>
<xml_diff>
--- a/data/测试集.xlsx
+++ b/data/测试集.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42253\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\program\pycharm\model\neural\土木\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F236AA05-4E66-42D5-8EB3-996C94F09D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A700E4-BE1F-4333-BCCA-E402E116121F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2288,60 +2288,72 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B55">
         <v>3</v>
       </c>
       <c r="C55">
-        <v>5.3259999999999996</v>
+        <v>17.331</v>
       </c>
       <c r="D55">
-        <v>6.09</v>
+        <v>9.1440000000000001</v>
       </c>
       <c r="E55">
-        <v>24.34</v>
+        <v>64.765000000000001</v>
       </c>
       <c r="F55">
-        <v>8.8230000000000004</v>
+        <v>23.913</v>
       </c>
       <c r="G55">
-        <v>6.64</v>
+        <v>7.88</v>
+      </c>
+      <c r="H55">
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="I55">
+        <v>14</v>
+      </c>
+      <c r="J55">
+        <v>0.436</v>
+      </c>
+      <c r="K55">
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>17.331</v>
+        <v>26.271999999999998</v>
       </c>
       <c r="D56">
-        <v>9.1440000000000001</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E56">
-        <v>64.765000000000001</v>
+        <v>31.588000000000001</v>
       </c>
       <c r="F56">
-        <v>23.913</v>
+        <v>6.5460000000000003</v>
       </c>
       <c r="G56">
-        <v>7.88</v>
+        <v>51.5</v>
       </c>
       <c r="H56">
-        <v>1.2490000000000001</v>
+        <v>1.5669999999999999</v>
       </c>
       <c r="I56">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J56">
-        <v>0.436</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="K56">
-        <v>174</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -2349,34 +2361,34 @@
         <v>2</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57">
-        <v>26.271999999999998</v>
+        <v>11.278</v>
       </c>
       <c r="D57">
-        <v>5.0999999999999996</v>
+        <v>11.8</v>
       </c>
       <c r="E57">
-        <v>31.588000000000001</v>
+        <v>104.738</v>
       </c>
       <c r="F57">
-        <v>6.5460000000000003</v>
+        <v>1.901</v>
       </c>
       <c r="G57">
-        <v>51.5</v>
+        <v>35.369999999999997</v>
       </c>
       <c r="H57">
-        <v>1.5669999999999999</v>
+        <v>1.742</v>
       </c>
       <c r="I57">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J57">
-        <v>8.7999999999999995E-2</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="K57">
-        <v>276</v>
+        <v>307</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
@@ -2387,31 +2399,31 @@
         <v>2</v>
       </c>
       <c r="C58">
-        <v>11.278</v>
+        <v>21.082000000000001</v>
       </c>
       <c r="D58">
-        <v>11.8</v>
+        <v>11.558</v>
       </c>
       <c r="E58">
-        <v>104.738</v>
+        <v>97.251000000000005</v>
       </c>
       <c r="F58">
-        <v>1.901</v>
+        <v>5.7649999999999997</v>
       </c>
       <c r="G58">
-        <v>35.369999999999997</v>
+        <v>30.98</v>
       </c>
       <c r="H58">
-        <v>1.742</v>
+        <v>1.847</v>
       </c>
       <c r="I58">
         <v>18</v>
       </c>
       <c r="J58">
-        <v>0.11899999999999999</v>
+        <v>0.124</v>
       </c>
       <c r="K58">
-        <v>307</v>
+        <v>364</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
@@ -2422,31 +2434,31 @@
         <v>2</v>
       </c>
       <c r="C59">
-        <v>21.082000000000001</v>
+        <v>11.086</v>
       </c>
       <c r="D59">
-        <v>11.558</v>
+        <v>9.9540000000000006</v>
       </c>
       <c r="E59">
-        <v>97.251000000000005</v>
+        <v>37.314</v>
       </c>
       <c r="F59">
-        <v>5.7649999999999997</v>
+        <v>17.488</v>
       </c>
       <c r="G59">
-        <v>30.98</v>
+        <v>29.43</v>
       </c>
       <c r="H59">
-        <v>1.847</v>
+        <v>1.7589999999999999</v>
       </c>
       <c r="I59">
         <v>18</v>
       </c>
       <c r="J59">
-        <v>0.124</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="K59">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
@@ -2457,31 +2469,31 @@
         <v>2</v>
       </c>
       <c r="C60">
-        <v>11.086</v>
+        <v>22.292000000000002</v>
       </c>
       <c r="D60">
-        <v>9.9540000000000006</v>
+        <v>11.714</v>
       </c>
       <c r="E60">
-        <v>37.314</v>
+        <v>76.165999999999997</v>
       </c>
       <c r="F60">
-        <v>17.488</v>
+        <v>23.195</v>
       </c>
       <c r="G60">
-        <v>29.43</v>
+        <v>22.71</v>
       </c>
       <c r="H60">
-        <v>1.7589999999999999</v>
+        <v>1.6</v>
       </c>
       <c r="I60">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J60">
-        <v>8.6999999999999994E-2</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="K60">
-        <v>367</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
@@ -2492,66 +2504,66 @@
         <v>2</v>
       </c>
       <c r="C61">
-        <v>22.292000000000002</v>
+        <v>23.292999999999999</v>
       </c>
       <c r="D61">
-        <v>11.714</v>
+        <v>10.481999999999999</v>
       </c>
       <c r="E61">
-        <v>76.165999999999997</v>
+        <v>97.031000000000006</v>
       </c>
       <c r="F61">
-        <v>23.195</v>
+        <v>25.844999999999999</v>
       </c>
       <c r="G61">
-        <v>22.71</v>
+        <v>26.11</v>
       </c>
       <c r="H61">
-        <v>1.6</v>
+        <v>1.8240000000000001</v>
       </c>
       <c r="I61">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J61">
-        <v>0.54100000000000004</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="K61">
-        <v>182</v>
+        <v>364</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>23.292999999999999</v>
+        <v>14.374000000000001</v>
       </c>
       <c r="D62">
-        <v>10.481999999999999</v>
+        <v>4.0439999999999996</v>
       </c>
       <c r="E62">
-        <v>97.031000000000006</v>
+        <v>27.94</v>
       </c>
       <c r="F62">
-        <v>25.844999999999999</v>
+        <v>7.1150000000000002</v>
       </c>
       <c r="G62">
-        <v>26.11</v>
+        <v>18.13</v>
       </c>
       <c r="H62">
-        <v>1.8240000000000001</v>
+        <v>1.6519999999999999</v>
       </c>
       <c r="I62">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J62">
-        <v>0.11600000000000001</v>
+        <v>0.108</v>
       </c>
       <c r="K62">
-        <v>364</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
@@ -2562,31 +2574,31 @@
         <v>3</v>
       </c>
       <c r="C63">
-        <v>14.374000000000001</v>
+        <v>15.497</v>
       </c>
       <c r="D63">
-        <v>4.0439999999999996</v>
+        <v>3.72</v>
       </c>
       <c r="E63">
-        <v>27.94</v>
+        <v>41.052999999999997</v>
       </c>
       <c r="F63">
-        <v>7.1150000000000002</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="G63">
-        <v>18.13</v>
+        <v>19.14</v>
       </c>
       <c r="H63">
-        <v>1.6519999999999999</v>
+        <v>1.7509999999999999</v>
       </c>
       <c r="I63">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J63">
-        <v>0.108</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="K63">
-        <v>170</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
@@ -2597,31 +2609,31 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <v>15.497</v>
+        <v>13.308999999999999</v>
       </c>
       <c r="D64">
-        <v>3.72</v>
+        <v>4.2619999999999996</v>
       </c>
       <c r="E64">
-        <v>41.052999999999997</v>
+        <v>36.747</v>
       </c>
       <c r="F64">
-        <v>9.2100000000000009</v>
+        <v>9.5589999999999993</v>
       </c>
       <c r="G64">
-        <v>19.14</v>
+        <v>24.56</v>
       </c>
       <c r="H64">
-        <v>1.7509999999999999</v>
+        <v>1.843</v>
       </c>
       <c r="I64">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J64">
-        <v>9.0999999999999998E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="K64">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
@@ -2632,31 +2644,31 @@
         <v>3</v>
       </c>
       <c r="C65">
-        <v>13.308999999999999</v>
+        <v>11.913</v>
       </c>
       <c r="D65">
-        <v>4.2619999999999996</v>
+        <v>2.8820000000000001</v>
       </c>
       <c r="E65">
-        <v>36.747</v>
+        <v>42.000999999999998</v>
       </c>
       <c r="F65">
-        <v>9.5589999999999993</v>
+        <v>9.4169999999999998</v>
       </c>
       <c r="G65">
-        <v>24.56</v>
+        <v>16.989999999999998</v>
       </c>
       <c r="H65">
-        <v>1.843</v>
+        <v>1.6040000000000001</v>
       </c>
       <c r="I65">
         <v>20</v>
       </c>
       <c r="J65">
-        <v>8.6999999999999994E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="K65">
-        <v>176</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
@@ -2667,31 +2679,31 @@
         <v>3</v>
       </c>
       <c r="C66">
-        <v>11.913</v>
+        <v>12.061</v>
       </c>
       <c r="D66">
-        <v>2.8820000000000001</v>
+        <v>4.0229999999999997</v>
       </c>
       <c r="E66">
-        <v>42.000999999999998</v>
+        <v>32.996000000000002</v>
       </c>
       <c r="F66">
-        <v>9.4169999999999998</v>
+        <v>5.5620000000000003</v>
       </c>
       <c r="G66">
-        <v>16.989999999999998</v>
+        <v>24.76</v>
       </c>
       <c r="H66">
-        <v>1.6040000000000001</v>
+        <v>1.6060000000000001</v>
       </c>
       <c r="I66">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J66">
-        <v>7.3999999999999996E-2</v>
+        <v>0.13</v>
       </c>
       <c r="K66">
-        <v>153</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
@@ -2702,31 +2714,31 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <v>12.061</v>
+        <v>13.993</v>
       </c>
       <c r="D67">
-        <v>4.0229999999999997</v>
+        <v>4.3150000000000004</v>
       </c>
       <c r="E67">
-        <v>32.996000000000002</v>
+        <v>33.1</v>
       </c>
       <c r="F67">
-        <v>5.5620000000000003</v>
+        <v>9.6649999999999991</v>
       </c>
       <c r="G67">
-        <v>24.76</v>
+        <v>21.45</v>
       </c>
       <c r="H67">
-        <v>1.6060000000000001</v>
+        <v>1.512</v>
       </c>
       <c r="I67">
         <v>18</v>
       </c>
       <c r="J67">
-        <v>0.13</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="K67">
-        <v>204</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -2734,34 +2746,34 @@
         <v>4</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>13.993</v>
+        <v>12.326000000000001</v>
       </c>
       <c r="D68">
-        <v>4.3150000000000004</v>
+        <v>4.7050000000000001</v>
       </c>
       <c r="E68">
-        <v>33.1</v>
+        <v>41.28</v>
       </c>
       <c r="F68">
-        <v>9.6649999999999991</v>
+        <v>9.218</v>
       </c>
       <c r="G68">
-        <v>21.45</v>
+        <v>16</v>
       </c>
       <c r="H68">
-        <v>1.512</v>
+        <v>1.722</v>
       </c>
       <c r="I68">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J68">
-        <v>9.2999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="K68">
-        <v>160</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
@@ -2772,31 +2784,31 @@
         <v>4</v>
       </c>
       <c r="C69">
-        <v>12.326000000000001</v>
+        <v>15.086</v>
       </c>
       <c r="D69">
-        <v>4.7050000000000001</v>
+        <v>2.8679999999999999</v>
       </c>
       <c r="E69">
-        <v>41.28</v>
+        <v>31.888000000000002</v>
       </c>
       <c r="F69">
-        <v>9.218</v>
+        <v>6.7510000000000003</v>
       </c>
       <c r="G69">
-        <v>16</v>
+        <v>17.55</v>
       </c>
       <c r="H69">
-        <v>1.722</v>
+        <v>1.6679999999999999</v>
       </c>
       <c r="I69">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J69">
-        <v>5.0999999999999997E-2</v>
+        <v>0.114</v>
       </c>
       <c r="K69">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
@@ -2807,28 +2819,28 @@
         <v>4</v>
       </c>
       <c r="C70">
-        <v>15.086</v>
+        <v>11.965</v>
       </c>
       <c r="D70">
-        <v>2.8679999999999999</v>
+        <v>3.911</v>
       </c>
       <c r="E70">
-        <v>31.888000000000002</v>
+        <v>32.439</v>
       </c>
       <c r="F70">
-        <v>6.7510000000000003</v>
+        <v>6.7480000000000002</v>
       </c>
       <c r="G70">
-        <v>17.55</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H70">
-        <v>1.6679999999999999</v>
+        <v>1.5169999999999999</v>
       </c>
       <c r="I70">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J70">
-        <v>0.114</v>
+        <v>0.128</v>
       </c>
       <c r="K70">
         <v>168</v>
@@ -2839,34 +2851,34 @@
         <v>4</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>11.965</v>
+        <v>12.006</v>
       </c>
       <c r="D71">
-        <v>3.911</v>
+        <v>2.7759999999999998</v>
       </c>
       <c r="E71">
-        <v>32.439</v>
+        <v>36.904000000000003</v>
       </c>
       <c r="F71">
-        <v>6.7480000000000002</v>
+        <v>5.7539999999999996</v>
       </c>
       <c r="G71">
-        <v>16.100000000000001</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="H71">
-        <v>1.5169999999999999</v>
+        <v>1.56</v>
       </c>
       <c r="I71">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J71">
-        <v>0.128</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="K71">
-        <v>168</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
@@ -2877,31 +2889,31 @@
         <v>3</v>
       </c>
       <c r="C72">
-        <v>12.006</v>
+        <v>10.853999999999999</v>
       </c>
       <c r="D72">
-        <v>2.7759999999999998</v>
+        <v>3.78</v>
       </c>
       <c r="E72">
-        <v>36.904000000000003</v>
+        <v>40.704999999999998</v>
       </c>
       <c r="F72">
-        <v>5.7539999999999996</v>
+        <v>7.96</v>
       </c>
       <c r="G72">
-        <v>18.600000000000001</v>
+        <v>25.82</v>
       </c>
       <c r="H72">
-        <v>1.56</v>
+        <v>1.756</v>
       </c>
       <c r="I72">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J72">
-        <v>6.6000000000000003E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="K72">
-        <v>190</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
@@ -2912,31 +2924,31 @@
         <v>3</v>
       </c>
       <c r="C73">
-        <v>10.853999999999999</v>
+        <v>10.944000000000001</v>
       </c>
       <c r="D73">
-        <v>3.78</v>
+        <v>4.6920000000000002</v>
       </c>
       <c r="E73">
-        <v>40.704999999999998</v>
+        <v>33.274000000000001</v>
       </c>
       <c r="F73">
-        <v>7.96</v>
+        <v>5.7450000000000001</v>
       </c>
       <c r="G73">
-        <v>25.82</v>
+        <v>17.77</v>
       </c>
       <c r="H73">
-        <v>1.756</v>
+        <v>1.5569999999999999</v>
       </c>
       <c r="I73">
         <v>20</v>
       </c>
       <c r="J73">
-        <v>8.2000000000000003E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="K73">
-        <v>152</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
@@ -2947,31 +2959,31 @@
         <v>3</v>
       </c>
       <c r="C74">
-        <v>10.944000000000001</v>
+        <v>10.853999999999999</v>
       </c>
       <c r="D74">
-        <v>4.6920000000000002</v>
+        <v>3.78</v>
       </c>
       <c r="E74">
-        <v>33.274000000000001</v>
+        <v>40.704999999999998</v>
       </c>
       <c r="F74">
-        <v>5.7450000000000001</v>
+        <v>7.96</v>
       </c>
       <c r="G74">
-        <v>17.77</v>
+        <v>25.82</v>
       </c>
       <c r="H74">
-        <v>1.5569999999999999</v>
+        <v>1.756</v>
       </c>
       <c r="I74">
         <v>20</v>
       </c>
       <c r="J74">
-        <v>6.2E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="K74">
-        <v>218</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
@@ -2982,66 +2994,66 @@
         <v>3</v>
       </c>
       <c r="C75">
-        <v>10.853999999999999</v>
+        <v>10.944000000000001</v>
       </c>
       <c r="D75">
-        <v>3.78</v>
+        <v>4.6920000000000002</v>
       </c>
       <c r="E75">
-        <v>40.704999999999998</v>
+        <v>33.274000000000001</v>
       </c>
       <c r="F75">
-        <v>7.96</v>
+        <v>5.7450000000000001</v>
       </c>
       <c r="G75">
-        <v>25.82</v>
+        <v>17.77</v>
       </c>
       <c r="H75">
-        <v>1.756</v>
+        <v>1.5569999999999999</v>
       </c>
       <c r="I75">
         <v>20</v>
       </c>
       <c r="J75">
-        <v>8.2000000000000003E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="K75">
-        <v>152</v>
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B76">
         <v>3</v>
       </c>
       <c r="C76">
-        <v>10.944000000000001</v>
+        <v>9.4290000000000003</v>
       </c>
       <c r="D76">
-        <v>4.6920000000000002</v>
+        <v>7.1269999999999998</v>
       </c>
       <c r="E76">
-        <v>33.274000000000001</v>
+        <v>59.786999999999999</v>
       </c>
       <c r="F76">
-        <v>5.7450000000000001</v>
+        <v>8.6180000000000003</v>
       </c>
       <c r="G76">
-        <v>17.77</v>
+        <v>38.44</v>
       </c>
       <c r="H76">
-        <v>1.5569999999999999</v>
+        <v>1.3120000000000001</v>
       </c>
       <c r="I76">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="J76">
-        <v>6.2E-2</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="K76">
-        <v>218</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
@@ -3052,31 +3064,31 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>9.4290000000000003</v>
+        <v>5.73</v>
       </c>
       <c r="D77">
-        <v>7.1269999999999998</v>
+        <v>7.3280000000000003</v>
       </c>
       <c r="E77">
-        <v>59.786999999999999</v>
+        <v>57.313000000000002</v>
       </c>
       <c r="F77">
-        <v>8.6180000000000003</v>
+        <v>7.76</v>
       </c>
       <c r="G77">
-        <v>38.44</v>
+        <v>36.619999999999997</v>
       </c>
       <c r="H77">
-        <v>1.3120000000000001</v>
+        <v>1.222</v>
       </c>
       <c r="I77">
         <v>11</v>
       </c>
       <c r="J77">
-        <v>0.20300000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="K77">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
@@ -3087,31 +3099,31 @@
         <v>3</v>
       </c>
       <c r="C78">
-        <v>5.73</v>
+        <v>10.324999999999999</v>
       </c>
       <c r="D78">
-        <v>7.3280000000000003</v>
+        <v>7.4</v>
       </c>
       <c r="E78">
-        <v>57.313000000000002</v>
+        <v>61.348999999999997</v>
       </c>
       <c r="F78">
-        <v>7.76</v>
+        <v>7.1840000000000002</v>
       </c>
       <c r="G78">
-        <v>36.619999999999997</v>
+        <v>28.29</v>
       </c>
       <c r="H78">
-        <v>1.222</v>
+        <v>1.2070000000000001</v>
       </c>
       <c r="I78">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J78">
-        <v>0.23</v>
+        <v>0.217</v>
       </c>
       <c r="K78">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
@@ -3122,66 +3134,66 @@
         <v>3</v>
       </c>
       <c r="C79">
-        <v>10.324999999999999</v>
+        <v>5.4720000000000004</v>
       </c>
       <c r="D79">
-        <v>7.4</v>
+        <v>5.89</v>
       </c>
       <c r="E79">
-        <v>61.348999999999997</v>
+        <v>49.197000000000003</v>
       </c>
       <c r="F79">
-        <v>7.1840000000000002</v>
+        <v>8.6750000000000007</v>
       </c>
       <c r="G79">
-        <v>28.29</v>
+        <v>38.770000000000003</v>
       </c>
       <c r="H79">
-        <v>1.2070000000000001</v>
+        <v>1.337</v>
       </c>
       <c r="I79">
         <v>12</v>
       </c>
       <c r="J79">
-        <v>0.217</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="K79">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B80">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C80">
-        <v>5.4720000000000004</v>
+        <v>13.54</v>
       </c>
       <c r="D80">
-        <v>5.89</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="E80">
-        <v>49.197000000000003</v>
+        <v>31.475999999999999</v>
       </c>
       <c r="F80">
-        <v>8.6750000000000007</v>
+        <v>7.9279999999999999</v>
       </c>
       <c r="G80">
-        <v>38.770000000000003</v>
+        <v>47.59</v>
       </c>
       <c r="H80">
-        <v>1.337</v>
+        <v>0.95</v>
       </c>
       <c r="I80">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J80">
-        <v>0.17499999999999999</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="K80">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
@@ -3192,66 +3204,66 @@
         <v>4</v>
       </c>
       <c r="C81">
-        <v>13.54</v>
+        <v>13.909000000000001</v>
       </c>
       <c r="D81">
-        <v>4.1500000000000004</v>
+        <v>3.9809999999999999</v>
       </c>
       <c r="E81">
-        <v>31.475999999999999</v>
+        <v>22.797000000000001</v>
       </c>
       <c r="F81">
-        <v>7.9279999999999999</v>
+        <v>11.603</v>
       </c>
       <c r="G81">
-        <v>47.59</v>
+        <v>48.11</v>
       </c>
       <c r="H81">
-        <v>0.95</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="I81">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J81">
-        <v>0.67600000000000005</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="K81">
-        <v>104</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B82">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>13.909000000000001</v>
+        <v>17.452999999999999</v>
       </c>
       <c r="D82">
-        <v>3.9809999999999999</v>
+        <v>2.9430000000000001</v>
       </c>
       <c r="E82">
-        <v>22.797000000000001</v>
+        <v>63.323999999999998</v>
       </c>
       <c r="F82">
-        <v>11.603</v>
+        <v>15.532</v>
       </c>
       <c r="G82">
-        <v>48.11</v>
+        <v>60.24</v>
       </c>
       <c r="H82">
-        <v>0.44400000000000001</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="I82">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J82">
-        <v>0.63800000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="K82">
-        <v>127</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
@@ -3259,34 +3271,34 @@
         <v>2</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C83">
-        <v>17.452999999999999</v>
+        <v>15.462</v>
       </c>
       <c r="D83">
-        <v>2.9430000000000001</v>
+        <v>2.8530000000000002</v>
       </c>
       <c r="E83">
-        <v>63.323999999999998</v>
+        <v>43.872999999999998</v>
       </c>
       <c r="F83">
-        <v>15.532</v>
+        <v>14.430999999999999</v>
       </c>
       <c r="G83">
-        <v>60.24</v>
+        <v>56.15</v>
       </c>
       <c r="H83">
-        <v>1.2250000000000001</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="I83">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J83">
-        <v>0.17799999999999999</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="K83">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
@@ -3294,69 +3306,69 @@
         <v>2</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84">
-        <v>15.462</v>
+        <v>13.465</v>
       </c>
       <c r="D84">
-        <v>2.8530000000000002</v>
+        <v>3.0979999999999999</v>
       </c>
       <c r="E84">
-        <v>43.872999999999998</v>
+        <v>45.353999999999999</v>
       </c>
       <c r="F84">
-        <v>14.430999999999999</v>
+        <v>13.239000000000001</v>
       </c>
       <c r="G84">
-        <v>56.15</v>
+        <v>57.36</v>
       </c>
       <c r="H84">
-        <v>1.4750000000000001</v>
+        <v>1.4910000000000001</v>
       </c>
       <c r="I84">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J84">
-        <v>0.24199999999999999</v>
+        <v>0.254</v>
       </c>
       <c r="K84">
-        <v>259</v>
+        <v>280</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C85">
-        <v>13.465</v>
+        <v>13.260999999999999</v>
       </c>
       <c r="D85">
-        <v>3.0979999999999999</v>
+        <v>5.8630000000000004</v>
       </c>
       <c r="E85">
-        <v>45.353999999999999</v>
+        <v>39.302</v>
       </c>
       <c r="F85">
-        <v>13.239000000000001</v>
+        <v>12.194000000000001</v>
       </c>
       <c r="G85">
-        <v>57.36</v>
+        <v>39.67</v>
       </c>
       <c r="H85">
-        <v>1.4910000000000001</v>
+        <v>1.355</v>
       </c>
       <c r="I85">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J85">
-        <v>0.254</v>
+        <v>0.376</v>
       </c>
       <c r="K85">
-        <v>280</v>
+        <v>235</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
@@ -3364,34 +3376,34 @@
         <v>3</v>
       </c>
       <c r="B86">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C86">
-        <v>13.260999999999999</v>
+        <v>7.74</v>
       </c>
       <c r="D86">
-        <v>5.8630000000000004</v>
+        <v>10.173</v>
       </c>
       <c r="E86">
-        <v>39.302</v>
+        <v>60.372999999999998</v>
       </c>
       <c r="F86">
-        <v>12.194000000000001</v>
+        <v>18.474</v>
       </c>
       <c r="G86">
-        <v>39.67</v>
+        <v>28.36</v>
       </c>
       <c r="H86">
-        <v>1.355</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="I86">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J86">
-        <v>0.376</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="K86">
-        <v>235</v>
+        <v>275</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
@@ -3402,31 +3414,31 @@
         <v>3</v>
       </c>
       <c r="C87">
-        <v>7.74</v>
+        <v>16.434000000000001</v>
       </c>
       <c r="D87">
-        <v>10.173</v>
+        <v>5.7590000000000003</v>
       </c>
       <c r="E87">
-        <v>60.372999999999998</v>
+        <v>84.082999999999998</v>
       </c>
       <c r="F87">
-        <v>18.474</v>
+        <v>21.100999999999999</v>
       </c>
       <c r="G87">
-        <v>28.36</v>
+        <v>27.37</v>
       </c>
       <c r="H87">
-        <v>1.4119999999999999</v>
+        <v>1.2430000000000001</v>
       </c>
       <c r="I87">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J87">
-        <v>0.26100000000000001</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="K87">
-        <v>275</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
@@ -3437,66 +3449,66 @@
         <v>3</v>
       </c>
       <c r="C88">
-        <v>16.434000000000001</v>
+        <v>9.6329999999999991</v>
       </c>
       <c r="D88">
-        <v>5.7590000000000003</v>
+        <v>7.4740000000000002</v>
       </c>
       <c r="E88">
-        <v>84.082999999999998</v>
+        <v>47.731999999999999</v>
       </c>
       <c r="F88">
-        <v>21.100999999999999</v>
+        <v>11.137</v>
       </c>
       <c r="G88">
-        <v>27.37</v>
+        <v>30.94</v>
       </c>
       <c r="H88">
-        <v>1.2430000000000001</v>
+        <v>1.161</v>
       </c>
       <c r="I88">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J88">
-        <v>0.33500000000000002</v>
+        <v>0.253</v>
       </c>
       <c r="K88">
-        <v>201</v>
+        <v>292</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89">
-        <v>9.6329999999999991</v>
+        <v>6.7389999999999999</v>
       </c>
       <c r="D89">
-        <v>7.4740000000000002</v>
+        <v>6.8780000000000001</v>
       </c>
       <c r="E89">
-        <v>47.731999999999999</v>
+        <v>61.515999999999998</v>
       </c>
       <c r="F89">
-        <v>11.137</v>
+        <v>21.806000000000001</v>
       </c>
       <c r="G89">
-        <v>30.94</v>
+        <v>31.79</v>
       </c>
       <c r="H89">
-        <v>1.161</v>
+        <v>1.4870000000000001</v>
       </c>
       <c r="I89">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J89">
-        <v>0.253</v>
+        <v>0.52</v>
       </c>
       <c r="K89">
-        <v>292</v>
+        <v>202</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
@@ -3504,139 +3516,139 @@
         <v>2</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C90">
-        <v>6.7389999999999999</v>
+        <v>13.938000000000001</v>
       </c>
       <c r="D90">
-        <v>6.8780000000000001</v>
+        <v>4.226</v>
       </c>
       <c r="E90">
-        <v>61.515999999999998</v>
+        <v>58.572000000000003</v>
       </c>
       <c r="F90">
-        <v>21.806000000000001</v>
+        <v>14.439</v>
       </c>
       <c r="G90">
-        <v>31.79</v>
+        <v>66.3</v>
       </c>
       <c r="H90">
-        <v>1.4870000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I90">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J90">
-        <v>0.52</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="K90">
-        <v>202</v>
+        <v>239</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C91">
-        <v>13.938000000000001</v>
+        <v>10.682</v>
       </c>
       <c r="D91">
-        <v>4.226</v>
+        <v>6.851</v>
       </c>
       <c r="E91">
-        <v>58.572000000000003</v>
+        <v>52.286000000000001</v>
       </c>
       <c r="F91">
-        <v>14.439</v>
+        <v>17.553000000000001</v>
       </c>
       <c r="G91">
-        <v>66.3</v>
+        <v>29.46</v>
       </c>
       <c r="H91">
-        <v>1.1399999999999999</v>
+        <v>1.4179999999999999</v>
       </c>
       <c r="I91">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J91">
-        <v>0.14199999999999999</v>
+        <v>0.32700000000000001</v>
       </c>
       <c r="K91">
-        <v>239</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B92">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92">
-        <v>10.682</v>
+        <v>18.606000000000002</v>
       </c>
       <c r="D92">
-        <v>6.851</v>
+        <v>12.247999999999999</v>
       </c>
       <c r="E92">
-        <v>52.286000000000001</v>
+        <v>99.415999999999997</v>
       </c>
       <c r="F92">
-        <v>17.553000000000001</v>
+        <v>7.1040000000000001</v>
       </c>
       <c r="G92">
-        <v>29.46</v>
+        <v>33.119999999999997</v>
       </c>
       <c r="H92">
-        <v>1.4179999999999999</v>
+        <v>1.71</v>
       </c>
       <c r="I92">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J92">
-        <v>0.32700000000000001</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="K92">
-        <v>189</v>
+        <v>306</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C93">
-        <v>18.606000000000002</v>
+        <v>16.59</v>
       </c>
       <c r="D93">
-        <v>12.247999999999999</v>
+        <v>8.2970000000000006</v>
       </c>
       <c r="E93">
-        <v>99.415999999999997</v>
+        <v>57.475000000000001</v>
       </c>
       <c r="F93">
-        <v>7.1040000000000001</v>
+        <v>24.948</v>
       </c>
       <c r="G93">
-        <v>33.119999999999997</v>
+        <v>25.9</v>
       </c>
       <c r="H93">
-        <v>1.71</v>
+        <v>1.35</v>
       </c>
       <c r="I93">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="J93">
-        <v>6.0999999999999999E-2</v>
+        <v>0.35</v>
       </c>
       <c r="K93">
-        <v>306</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
@@ -3647,100 +3659,65 @@
         <v>3</v>
       </c>
       <c r="C94">
-        <v>16.59</v>
+        <v>17.331</v>
       </c>
       <c r="D94">
-        <v>8.2970000000000006</v>
+        <v>9.1440000000000001</v>
       </c>
       <c r="E94">
-        <v>57.475000000000001</v>
+        <v>64.765000000000001</v>
       </c>
       <c r="F94">
-        <v>24.948</v>
+        <v>23.913</v>
       </c>
       <c r="G94">
-        <v>25.9</v>
+        <v>7.88</v>
       </c>
       <c r="H94">
-        <v>1.35</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="I94">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J94">
-        <v>0.35</v>
+        <v>0.436</v>
       </c>
       <c r="K94">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B95">
         <v>3</v>
       </c>
       <c r="C95">
-        <v>17.331</v>
+        <v>13.308999999999999</v>
       </c>
       <c r="D95">
-        <v>9.1440000000000001</v>
+        <v>4.2619999999999996</v>
       </c>
       <c r="E95">
-        <v>64.765000000000001</v>
+        <v>36.747</v>
       </c>
       <c r="F95">
-        <v>23.913</v>
+        <v>9.5589999999999993</v>
       </c>
       <c r="G95">
-        <v>7.88</v>
+        <v>24.56</v>
       </c>
       <c r="H95">
-        <v>1.2490000000000001</v>
+        <v>1.843</v>
       </c>
       <c r="I95">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J95">
-        <v>0.436</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="K95">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>4</v>
-      </c>
-      <c r="B96">
-        <v>3</v>
-      </c>
-      <c r="C96">
-        <v>13.308999999999999</v>
-      </c>
-      <c r="D96">
-        <v>4.2619999999999996</v>
-      </c>
-      <c r="E96">
-        <v>36.747</v>
-      </c>
-      <c r="F96">
-        <v>9.5589999999999993</v>
-      </c>
-      <c r="G96">
-        <v>24.56</v>
-      </c>
-      <c r="H96">
-        <v>1.843</v>
-      </c>
-      <c r="I96">
-        <v>20</v>
-      </c>
-      <c r="J96">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="K96">
         <v>176</v>
       </c>
     </row>

</xml_diff>